<commit_message>
tens of bug fixes, one operand working fully
</commit_message>
<xml_diff>
--- a/opCodes.xlsx
+++ b/opCodes.xlsx
@@ -5,17 +5,20 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Files\College\Spring 2021\Computer Arch\Project\Repo\CMPN301-Project\CMPN301-PipelinedHarvardProcessor\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Uni\Sem6\CMPN301 Computer Architecture\Project\CMPN301-PipelinedHarvardProcessor\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{42FA3AE0-D249-4150-812D-CC352A3029A5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FBB10513-F2FA-4667-B173-5126B952D3CB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" activeTab="1" xr2:uid="{28913183-C242-4228-B8FD-946A1A5F0E6C}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" activeTab="1" xr2:uid="{28913183-C242-4228-B8FD-946A1A5F0E6C}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
     <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
   </sheets>
+  <definedNames>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="1" hidden="1">Sheet2!$A$1:$R$1</definedName>
+  </definedNames>
   <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
@@ -35,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="350" uniqueCount="113">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="350" uniqueCount="114">
   <si>
     <t>NOP</t>
   </si>
@@ -374,6 +377,9 @@
   </si>
   <si>
     <t>1111</t>
+  </si>
+  <si>
+    <t>0011</t>
   </si>
 </sst>
 </file>
@@ -734,40 +740,40 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F2ED3482-9716-4402-9EBD-931DDB0A284D}">
   <dimension ref="A1:I45"/>
   <sheetViews>
-    <sheetView topLeftCell="A4" workbookViewId="0">
-      <selection activeCell="E9" sqref="E9"/>
+    <sheetView topLeftCell="A33" workbookViewId="0">
+      <selection activeCell="B11" sqref="B11"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.109375" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="10" style="1" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="8.44140625" style="1" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="8.42578125" style="1" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="12" style="1" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="9" style="1" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="6" style="1" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="6.6640625" style="1" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="6.7109375" style="1" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="7" style="1" bestFit="1" customWidth="1"/>
-    <col min="8" max="9" width="5.44140625" style="1" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="10.5546875" style="1" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="11.44140625" style="1" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="13.6640625" style="1" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="9.88671875" style="1" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="17.88671875" style="1" bestFit="1" customWidth="1"/>
+    <col min="8" max="9" width="5.42578125" style="1" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="10.5703125" style="1" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="11.42578125" style="1" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="13.7109375" style="1" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="9.85546875" style="1" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="17.85546875" style="1" bestFit="1" customWidth="1"/>
     <col min="15" max="15" width="10" style="1" bestFit="1" customWidth="1"/>
-    <col min="16" max="16" width="10.5546875" style="1" bestFit="1" customWidth="1"/>
-    <col min="17" max="17" width="11.44140625" style="1" bestFit="1" customWidth="1"/>
-    <col min="18" max="18" width="13.6640625" style="1" bestFit="1" customWidth="1"/>
-    <col min="19" max="19" width="9.88671875" style="1" bestFit="1" customWidth="1"/>
-    <col min="20" max="20" width="7.6640625" style="1" bestFit="1" customWidth="1"/>
-    <col min="21" max="16384" width="9.109375" style="1"/>
+    <col min="16" max="16" width="10.5703125" style="1" bestFit="1" customWidth="1"/>
+    <col min="17" max="17" width="11.42578125" style="1" bestFit="1" customWidth="1"/>
+    <col min="18" max="18" width="13.7109375" style="1" bestFit="1" customWidth="1"/>
+    <col min="19" max="19" width="9.85546875" style="1" bestFit="1" customWidth="1"/>
+    <col min="20" max="20" width="7.7109375" style="1" bestFit="1" customWidth="1"/>
+    <col min="21" max="16384" width="9.140625" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:9" x14ac:dyDescent="0.25">
       <c r="H1" s="1" t="s">
         <v>78</v>
       </c>
     </row>
-    <row r="2" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
         <v>53</v>
       </c>
@@ -778,7 +784,7 @@
         <v>59</v>
       </c>
     </row>
-    <row r="3" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:9" x14ac:dyDescent="0.25">
       <c r="B3" s="1" t="s">
         <v>55</v>
       </c>
@@ -786,7 +792,7 @@
         <v>68</v>
       </c>
     </row>
-    <row r="4" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A4" s="1" t="s">
         <v>0</v>
       </c>
@@ -797,7 +803,7 @@
         <v>71</v>
       </c>
     </row>
-    <row r="5" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A5" s="1" t="s">
         <v>69</v>
       </c>
@@ -808,7 +814,7 @@
         <v>71</v>
       </c>
     </row>
-    <row r="6" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A6" s="1" t="s">
         <v>1</v>
       </c>
@@ -819,7 +825,7 @@
         <v>71</v>
       </c>
     </row>
-    <row r="7" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A7" s="1" t="s">
         <v>2</v>
       </c>
@@ -830,7 +836,7 @@
         <v>71</v>
       </c>
     </row>
-    <row r="9" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A9" s="1" t="s">
         <v>53</v>
       </c>
@@ -847,7 +853,7 @@
         <v>59</v>
       </c>
     </row>
-    <row r="10" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:9" x14ac:dyDescent="0.25">
       <c r="B10" s="1" t="s">
         <v>55</v>
       </c>
@@ -861,7 +867,7 @@
         <v>55</v>
       </c>
     </row>
-    <row r="11" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A11" s="1" t="s">
         <v>7</v>
       </c>
@@ -878,7 +884,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="12" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A12" s="1" t="s">
         <v>8</v>
       </c>
@@ -901,7 +907,7 @@
         <v>57</v>
       </c>
     </row>
-    <row r="13" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A13" s="1" t="s">
         <v>10</v>
       </c>
@@ -924,7 +930,7 @@
         <v>57</v>
       </c>
     </row>
-    <row r="14" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A14" s="1" t="s">
         <v>12</v>
       </c>
@@ -947,7 +953,7 @@
         <v>57</v>
       </c>
     </row>
-    <row r="15" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A15" s="1" t="s">
         <v>14</v>
       </c>
@@ -970,7 +976,7 @@
         <v>57</v>
       </c>
     </row>
-    <row r="17" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A17" s="1" t="s">
         <v>53</v>
       </c>
@@ -987,7 +993,7 @@
         <v>66</v>
       </c>
     </row>
-    <row r="18" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:9" x14ac:dyDescent="0.25">
       <c r="B18" s="1" t="s">
         <v>55</v>
       </c>
@@ -1001,7 +1007,7 @@
         <v>55</v>
       </c>
     </row>
-    <row r="19" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A19" s="1" t="s">
         <v>44</v>
       </c>
@@ -1024,7 +1030,7 @@
         <v>66</v>
       </c>
     </row>
-    <row r="20" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A20" s="1" t="s">
         <v>46</v>
       </c>
@@ -1047,7 +1053,7 @@
         <v>66</v>
       </c>
     </row>
-    <row r="22" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A22" s="1" t="s">
         <v>53</v>
       </c>
@@ -1061,7 +1067,7 @@
         <v>59</v>
       </c>
     </row>
-    <row r="23" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:9" x14ac:dyDescent="0.25">
       <c r="B23" s="1" t="s">
         <v>55</v>
       </c>
@@ -1072,7 +1078,7 @@
         <v>70</v>
       </c>
     </row>
-    <row r="24" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A24" s="1" t="s">
         <v>20</v>
       </c>
@@ -1086,7 +1092,7 @@
         <v>72</v>
       </c>
     </row>
-    <row r="25" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A25" s="1" t="s">
         <v>22</v>
       </c>
@@ -1103,7 +1109,7 @@
         <v>56</v>
       </c>
     </row>
-    <row r="26" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A26" s="1" t="s">
         <v>24</v>
       </c>
@@ -1120,7 +1126,7 @@
         <v>56</v>
       </c>
     </row>
-    <row r="27" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A27" s="1" t="s">
         <v>26</v>
       </c>
@@ -1137,7 +1143,7 @@
         <v>56</v>
       </c>
     </row>
-    <row r="28" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A28" s="1" t="s">
         <v>28</v>
       </c>
@@ -1151,7 +1157,7 @@
         <v>72</v>
       </c>
     </row>
-    <row r="29" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A29" s="1" t="s">
         <v>30</v>
       </c>
@@ -1165,7 +1171,7 @@
         <v>72</v>
       </c>
     </row>
-    <row r="30" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="30" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A30" s="1" t="s">
         <v>32</v>
       </c>
@@ -1179,7 +1185,7 @@
         <v>72</v>
       </c>
     </row>
-    <row r="31" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="31" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A31" s="1" t="s">
         <v>34</v>
       </c>
@@ -1193,7 +1199,7 @@
         <v>72</v>
       </c>
     </row>
-    <row r="32" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="32" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A32" s="1" t="s">
         <v>36</v>
       </c>
@@ -1207,7 +1213,7 @@
         <v>72</v>
       </c>
     </row>
-    <row r="33" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="33" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A33" s="1" t="s">
         <v>38</v>
       </c>
@@ -1221,7 +1227,7 @@
         <v>72</v>
       </c>
     </row>
-    <row r="34" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="34" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A34" s="1" t="s">
         <v>40</v>
       </c>
@@ -1235,7 +1241,7 @@
         <v>72</v>
       </c>
     </row>
-    <row r="35" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="35" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A35" s="1" t="s">
         <v>42</v>
       </c>
@@ -1249,7 +1255,7 @@
         <v>72</v>
       </c>
     </row>
-    <row r="37" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="37" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A37" s="1" t="s">
         <v>53</v>
       </c>
@@ -1269,7 +1275,7 @@
         <v>67</v>
       </c>
     </row>
-    <row r="38" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="38" spans="1:9" x14ac:dyDescent="0.25">
       <c r="B38" s="1" t="s">
         <v>55</v>
       </c>
@@ -1286,7 +1292,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="39" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="39" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A39" s="1" t="s">
         <v>16</v>
       </c>
@@ -1312,7 +1318,7 @@
         <v>67</v>
       </c>
     </row>
-    <row r="40" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="40" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A40" s="1" t="s">
         <v>18</v>
       </c>
@@ -1338,7 +1344,7 @@
         <v>67</v>
       </c>
     </row>
-    <row r="42" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="42" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A42" s="1" t="s">
         <v>53</v>
       </c>
@@ -1358,7 +1364,7 @@
         <v>66</v>
       </c>
     </row>
-    <row r="43" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="43" spans="1:9" x14ac:dyDescent="0.25">
       <c r="B43" s="1" t="s">
         <v>55</v>
       </c>
@@ -1375,7 +1381,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="44" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="44" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A44" s="1" t="s">
         <v>48</v>
       </c>
@@ -1401,7 +1407,7 @@
         <v>66</v>
       </c>
     </row>
-    <row r="45" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="45" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A45" s="1" t="s">
         <v>50</v>
       </c>
@@ -1432,25 +1438,25 @@
   <dimension ref="A1:R40"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
-      <selection activeCell="E27" sqref="E27"/>
+      <selection activeCell="E23" sqref="E23"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="10.5546875" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="8.44140625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="9.33203125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="10.5703125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="8.42578125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="9.28515625" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="7" style="1" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="11" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="7.109375" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="10.5546875" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="7.140625" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="10.5703125" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="10" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="7.6640625" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="7.5546875" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="9.88671875" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="7.7109375" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="7.5703125" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="9.85546875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:18" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>79</v>
       </c>
@@ -1503,7 +1509,7 @@
         <v>111</v>
       </c>
     </row>
-    <row r="2" spans="1:18" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
         <v>0</v>
       </c>
@@ -1541,18 +1547,18 @@
         <v>0</v>
       </c>
     </row>
-    <row r="3" spans="1:18" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
-        <v>69</v>
+        <v>2</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>3</v>
+        <v>6</v>
       </c>
       <c r="C3">
         <v>0</v>
       </c>
       <c r="E3" s="1" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="F3" t="s">
         <v>59</v>
@@ -1561,39 +1567,36 @@
         <v>0</v>
       </c>
       <c r="H3">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="I3">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="K3">
         <v>0</v>
       </c>
       <c r="L3">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="M3">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="N3">
         <v>0</v>
       </c>
-      <c r="Q3" t="s">
-        <v>97</v>
-      </c>
-    </row>
-    <row r="4" spans="1:18" x14ac:dyDescent="0.3">
+    </row>
+    <row r="4" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A4" s="1" t="s">
-        <v>1</v>
+        <v>28</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>5</v>
+        <v>29</v>
       </c>
       <c r="C4">
         <v>0</v>
       </c>
       <c r="E4" s="1" t="s">
-        <v>100</v>
+        <v>98</v>
       </c>
       <c r="F4" t="s">
         <v>59</v>
@@ -1614,77 +1617,77 @@
         <v>0</v>
       </c>
       <c r="M4">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="N4">
         <v>0</v>
       </c>
-      <c r="Q4" t="s">
-        <v>97</v>
-      </c>
-    </row>
-    <row r="5" spans="1:18" x14ac:dyDescent="0.3">
+    </row>
+    <row r="5" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A5" s="1" t="s">
-        <v>2</v>
+        <v>30</v>
       </c>
       <c r="B5" s="1" t="s">
-        <v>6</v>
+        <v>31</v>
       </c>
       <c r="C5">
-        <v>0</v>
+        <v>1</v>
+      </c>
+      <c r="D5" s="1" t="s">
+        <v>84</v>
       </c>
       <c r="E5" s="1" t="s">
+        <v>113</v>
+      </c>
+      <c r="F5" t="s">
+        <v>62</v>
+      </c>
+      <c r="G5">
+        <v>0</v>
+      </c>
+      <c r="H5">
+        <v>0</v>
+      </c>
+      <c r="I5">
+        <v>0</v>
+      </c>
+      <c r="K5">
+        <v>0</v>
+      </c>
+      <c r="L5">
+        <v>0</v>
+      </c>
+      <c r="M5">
+        <v>0</v>
+      </c>
+      <c r="N5">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="6" spans="1:18" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A6" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="B6" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="C6">
+        <v>0</v>
+      </c>
+      <c r="E6" s="1" t="s">
         <v>98</v>
       </c>
-      <c r="F5" t="s">
+      <c r="F6" t="s">
         <v>59</v>
       </c>
-      <c r="G5">
-        <v>0</v>
-      </c>
-      <c r="H5">
-        <v>1</v>
-      </c>
-      <c r="I5">
-        <v>1</v>
-      </c>
-      <c r="K5">
-        <v>0</v>
-      </c>
-      <c r="L5">
-        <v>1</v>
-      </c>
-      <c r="M5">
-        <v>0</v>
-      </c>
-      <c r="N5">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="6" spans="1:18" ht="15" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A6" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="B6" s="1" t="s">
-        <v>52</v>
-      </c>
-      <c r="C6">
-        <v>1</v>
-      </c>
-      <c r="E6" s="1" t="s">
-        <v>110</v>
-      </c>
-      <c r="F6" t="s">
-        <v>62</v>
-      </c>
       <c r="G6">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H6">
         <v>0</v>
       </c>
       <c r="I6">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="K6">
         <v>0</v>
@@ -1698,25 +1701,19 @@
       <c r="N6">
         <v>0</v>
       </c>
-      <c r="Q6" t="s">
-        <v>97</v>
-      </c>
-    </row>
-    <row r="7" spans="1:18" x14ac:dyDescent="0.3">
+    </row>
+    <row r="7" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A7" s="1" t="s">
-        <v>8</v>
+        <v>34</v>
       </c>
       <c r="B7" s="1" t="s">
-        <v>9</v>
+        <v>35</v>
       </c>
       <c r="C7">
         <v>1</v>
       </c>
-      <c r="D7" s="1" t="s">
-        <v>87</v>
-      </c>
       <c r="E7" s="1" t="s">
-        <v>108</v>
+        <v>98</v>
       </c>
       <c r="F7" t="s">
         <v>62</v>
@@ -1725,13 +1722,13 @@
         <v>0</v>
       </c>
       <c r="H7">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="I7">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="K7">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="L7">
         <v>0</v>
@@ -1742,28 +1739,22 @@
       <c r="N7">
         <v>0</v>
       </c>
-      <c r="Q7" t="s">
-        <v>97</v>
-      </c>
-    </row>
-    <row r="8" spans="1:18" x14ac:dyDescent="0.3">
+    </row>
+    <row r="8" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A8" s="1" t="s">
-        <v>10</v>
+        <v>36</v>
       </c>
       <c r="B8" s="1" t="s">
-        <v>11</v>
+        <v>37</v>
       </c>
       <c r="C8">
-        <v>1</v>
-      </c>
-      <c r="D8" s="1" t="s">
-        <v>87</v>
+        <v>0</v>
       </c>
       <c r="E8" s="1" t="s">
-        <v>109</v>
+        <v>98</v>
       </c>
       <c r="F8" t="s">
-        <v>62</v>
+        <v>59</v>
       </c>
       <c r="G8">
         <v>0</v>
@@ -1784,30 +1775,27 @@
         <v>0</v>
       </c>
       <c r="N8">
-        <v>0</v>
-      </c>
-      <c r="Q8" t="s">
-        <v>97</v>
-      </c>
-    </row>
-    <row r="9" spans="1:18" x14ac:dyDescent="0.3">
+        <v>1</v>
+      </c>
+      <c r="O8" t="s">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="9" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A9" s="1" t="s">
-        <v>12</v>
+        <v>38</v>
       </c>
       <c r="B9" s="1" t="s">
-        <v>13</v>
+        <v>39</v>
       </c>
       <c r="C9">
-        <v>1</v>
-      </c>
-      <c r="D9" s="1" t="s">
-        <v>87</v>
+        <v>0</v>
       </c>
       <c r="E9" s="1" t="s">
-        <v>101</v>
+        <v>98</v>
       </c>
       <c r="F9" t="s">
-        <v>62</v>
+        <v>59</v>
       </c>
       <c r="G9">
         <v>0</v>
@@ -1828,30 +1816,27 @@
         <v>0</v>
       </c>
       <c r="N9">
-        <v>0</v>
-      </c>
-      <c r="Q9" t="s">
-        <v>97</v>
-      </c>
-    </row>
-    <row r="10" spans="1:18" x14ac:dyDescent="0.3">
+        <v>1</v>
+      </c>
+      <c r="O9" t="s">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="10" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A10" s="1" t="s">
-        <v>14</v>
+        <v>40</v>
       </c>
       <c r="B10" s="1" t="s">
-        <v>15</v>
+        <v>41</v>
       </c>
       <c r="C10">
-        <v>1</v>
-      </c>
-      <c r="D10" s="1" t="s">
-        <v>87</v>
+        <v>0</v>
       </c>
       <c r="E10" s="1" t="s">
-        <v>102</v>
+        <v>98</v>
       </c>
       <c r="F10" t="s">
-        <v>62</v>
+        <v>59</v>
       </c>
       <c r="G10">
         <v>0</v>
@@ -1872,30 +1857,27 @@
         <v>0</v>
       </c>
       <c r="N10">
-        <v>0</v>
-      </c>
-      <c r="Q10" t="s">
-        <v>97</v>
-      </c>
-    </row>
-    <row r="11" spans="1:18" x14ac:dyDescent="0.3">
+        <v>1</v>
+      </c>
+      <c r="O10" t="s">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="11" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A11" s="1" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="B11" s="1" t="s">
-        <v>17</v>
+        <v>43</v>
       </c>
       <c r="C11">
-        <v>1</v>
-      </c>
-      <c r="D11" s="1" t="s">
-        <v>86</v>
+        <v>0</v>
       </c>
       <c r="E11" s="1" t="s">
-        <v>103</v>
+        <v>98</v>
       </c>
       <c r="F11" t="s">
-        <v>62</v>
+        <v>59</v>
       </c>
       <c r="G11">
         <v>0</v>
@@ -1916,30 +1898,27 @@
         <v>0</v>
       </c>
       <c r="N11">
-        <v>0</v>
-      </c>
-      <c r="P11" t="s">
-        <v>94</v>
-      </c>
-      <c r="Q11" t="s">
-        <v>97</v>
-      </c>
-    </row>
-    <row r="12" spans="1:18" x14ac:dyDescent="0.3">
+        <v>1</v>
+      </c>
+      <c r="O11" t="s">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="12" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A12" s="1" t="s">
-        <v>46</v>
+        <v>16</v>
       </c>
       <c r="B12" s="1" t="s">
-        <v>19</v>
+        <v>45</v>
       </c>
       <c r="C12">
         <v>1</v>
       </c>
       <c r="D12" s="1" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="E12" s="1" t="s">
-        <v>104</v>
+        <v>98</v>
       </c>
       <c r="F12" t="s">
         <v>62</v>
@@ -1948,13 +1927,13 @@
         <v>0</v>
       </c>
       <c r="H12">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="I12">
         <v>0</v>
       </c>
       <c r="K12">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="L12">
         <v>0</v>
@@ -1966,25 +1945,24 @@
         <v>0</v>
       </c>
       <c r="P12" t="s">
-        <v>94</v>
-      </c>
-      <c r="Q12" t="s">
-        <v>97</v>
-      </c>
-    </row>
-    <row r="13" spans="1:18" x14ac:dyDescent="0.3">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="13" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A13" s="1" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="B13" s="1" t="s">
-        <v>21</v>
+        <v>47</v>
       </c>
       <c r="C13">
         <v>0</v>
       </c>
-      <c r="E13" s="1" t="str">
-        <f>B13</f>
-        <v>10000</v>
+      <c r="D13" s="1" t="s">
+        <v>85</v>
+      </c>
+      <c r="E13" s="1" t="s">
+        <v>98</v>
       </c>
       <c r="F13" t="s">
         <v>59</v>
@@ -1996,13 +1974,13 @@
         <v>0</v>
       </c>
       <c r="I13">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="K13">
         <v>0</v>
       </c>
       <c r="L13">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="M13">
         <v>0</v>
@@ -2010,19 +1988,25 @@
       <c r="N13">
         <v>0</v>
       </c>
-    </row>
-    <row r="14" spans="1:18" x14ac:dyDescent="0.3">
+      <c r="P13" t="s">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="14" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A14" s="1" t="s">
-        <v>22</v>
+        <v>50</v>
       </c>
       <c r="B14" s="1" t="s">
-        <v>23</v>
+        <v>51</v>
       </c>
       <c r="C14">
         <v>1</v>
       </c>
+      <c r="D14" s="1" t="s">
+        <v>85</v>
+      </c>
       <c r="E14" s="1" t="s">
-        <v>107</v>
+        <v>98</v>
       </c>
       <c r="F14" t="s">
         <v>62</v>
@@ -2048,25 +2032,25 @@
       <c r="N14">
         <v>0</v>
       </c>
-      <c r="Q14" t="s">
-        <v>97</v>
-      </c>
-    </row>
-    <row r="15" spans="1:18" x14ac:dyDescent="0.3">
+      <c r="P14" t="s">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="15" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A15" s="1" t="s">
-        <v>24</v>
+        <v>69</v>
       </c>
       <c r="B15" s="1" t="s">
-        <v>25</v>
+        <v>3</v>
       </c>
       <c r="C15">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E15" s="1" t="s">
-        <v>105</v>
+        <v>99</v>
       </c>
       <c r="F15" t="s">
-        <v>62</v>
+        <v>59</v>
       </c>
       <c r="G15">
         <v>0</v>
@@ -2084,7 +2068,7 @@
         <v>0</v>
       </c>
       <c r="M15">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="N15">
         <v>0</v>
@@ -2093,21 +2077,21 @@
         <v>97</v>
       </c>
     </row>
-    <row r="16" spans="1:18" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A16" s="1" t="s">
-        <v>26</v>
+        <v>1</v>
       </c>
       <c r="B16" s="1" t="s">
-        <v>27</v>
+        <v>5</v>
       </c>
       <c r="C16">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E16" s="1" t="s">
-        <v>106</v>
+        <v>100</v>
       </c>
       <c r="F16" t="s">
-        <v>62</v>
+        <v>59</v>
       </c>
       <c r="G16">
         <v>0</v>
@@ -2125,7 +2109,7 @@
         <v>0</v>
       </c>
       <c r="M16">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="N16">
         <v>0</v>
@@ -2134,21 +2118,24 @@
         <v>97</v>
       </c>
     </row>
-    <row r="17" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A17" s="1" t="s">
-        <v>28</v>
+        <v>12</v>
       </c>
       <c r="B17" s="1" t="s">
-        <v>29</v>
+        <v>13</v>
       </c>
       <c r="C17">
-        <v>0</v>
+        <v>1</v>
+      </c>
+      <c r="D17" s="1" t="s">
+        <v>87</v>
       </c>
       <c r="E17" s="1" t="s">
-        <v>98</v>
+        <v>101</v>
       </c>
       <c r="F17" t="s">
-        <v>59</v>
+        <v>62</v>
       </c>
       <c r="G17">
         <v>0</v>
@@ -2171,22 +2158,25 @@
       <c r="N17">
         <v>0</v>
       </c>
-    </row>
-    <row r="18" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="Q17" t="s">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="18" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A18" s="1" t="s">
-        <v>30</v>
+        <v>14</v>
       </c>
       <c r="B18" s="1" t="s">
-        <v>31</v>
+        <v>15</v>
       </c>
       <c r="C18">
         <v>1</v>
       </c>
       <c r="D18" s="1" t="s">
-        <v>84</v>
+        <v>87</v>
       </c>
       <c r="E18" s="1" t="s">
-        <v>98</v>
+        <v>102</v>
       </c>
       <c r="F18" t="s">
         <v>62</v>
@@ -2212,31 +2202,34 @@
       <c r="N18">
         <v>0</v>
       </c>
-    </row>
-    <row r="19" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="Q18" t="s">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="19" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A19" s="1" t="s">
-        <v>32</v>
+        <v>22</v>
       </c>
       <c r="B19" s="1" t="s">
-        <v>33</v>
+        <v>23</v>
       </c>
       <c r="C19">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E19" s="1" t="s">
-        <v>98</v>
+        <v>107</v>
       </c>
       <c r="F19" t="s">
-        <v>59</v>
+        <v>62</v>
       </c>
       <c r="G19">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="H19">
         <v>0</v>
       </c>
       <c r="I19">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="K19">
         <v>0</v>
@@ -2250,19 +2243,25 @@
       <c r="N19">
         <v>0</v>
       </c>
-    </row>
-    <row r="20" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="Q19" t="s">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="20" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A20" s="1" t="s">
-        <v>34</v>
+        <v>44</v>
       </c>
       <c r="B20" s="1" t="s">
-        <v>35</v>
+        <v>17</v>
       </c>
       <c r="C20">
         <v>1</v>
       </c>
+      <c r="D20" s="1" t="s">
+        <v>86</v>
+      </c>
       <c r="E20" s="1" t="s">
-        <v>98</v>
+        <v>103</v>
       </c>
       <c r="F20" t="s">
         <v>62</v>
@@ -2271,13 +2270,13 @@
         <v>0</v>
       </c>
       <c r="H20">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="I20">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="K20">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="L20">
         <v>0</v>
@@ -2288,63 +2287,70 @@
       <c r="N20">
         <v>0</v>
       </c>
-    </row>
-    <row r="21" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="P20" t="s">
+        <v>94</v>
+      </c>
+      <c r="Q20" t="s">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="21" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A21" s="1" t="s">
-        <v>36</v>
+        <v>20</v>
       </c>
       <c r="B21" s="1" t="s">
-        <v>37</v>
+        <v>21</v>
       </c>
       <c r="C21">
         <v>0</v>
       </c>
-      <c r="E21" s="1" t="s">
-        <v>98</v>
+      <c r="E21" s="1" t="str">
+        <f>B21</f>
+        <v>10000</v>
       </c>
       <c r="F21" t="s">
         <v>59</v>
       </c>
       <c r="G21">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H21">
         <v>0</v>
       </c>
       <c r="I21">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="K21">
         <v>0</v>
       </c>
       <c r="L21">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="M21">
         <v>0</v>
       </c>
       <c r="N21">
-        <v>1</v>
-      </c>
-      <c r="O21" t="s">
-        <v>92</v>
-      </c>
-    </row>
-    <row r="22" spans="1:16" x14ac:dyDescent="0.3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="22" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A22" s="1" t="s">
-        <v>38</v>
+        <v>46</v>
       </c>
       <c r="B22" s="1" t="s">
-        <v>39</v>
+        <v>19</v>
       </c>
       <c r="C22">
-        <v>0</v>
+        <v>1</v>
+      </c>
+      <c r="D22" s="1" t="s">
+        <v>86</v>
       </c>
       <c r="E22" s="1" t="s">
-        <v>98</v>
+        <v>104</v>
       </c>
       <c r="F22" t="s">
-        <v>59</v>
+        <v>62</v>
       </c>
       <c r="G22">
         <v>0</v>
@@ -2365,27 +2371,30 @@
         <v>0</v>
       </c>
       <c r="N22">
-        <v>1</v>
-      </c>
-      <c r="O22" t="s">
-        <v>93</v>
-      </c>
-    </row>
-    <row r="23" spans="1:16" x14ac:dyDescent="0.3">
+        <v>0</v>
+      </c>
+      <c r="P22" t="s">
+        <v>94</v>
+      </c>
+      <c r="Q22" t="s">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="23" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A23" s="1" t="s">
-        <v>40</v>
+        <v>24</v>
       </c>
       <c r="B23" s="1" t="s">
-        <v>41</v>
+        <v>25</v>
       </c>
       <c r="C23">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E23" s="1" t="s">
-        <v>98</v>
+        <v>105</v>
       </c>
       <c r="F23" t="s">
-        <v>59</v>
+        <v>62</v>
       </c>
       <c r="G23">
         <v>0</v>
@@ -2406,27 +2415,27 @@
         <v>0</v>
       </c>
       <c r="N23">
-        <v>1</v>
-      </c>
-      <c r="O23" t="s">
-        <v>94</v>
-      </c>
-    </row>
-    <row r="24" spans="1:16" x14ac:dyDescent="0.3">
+        <v>0</v>
+      </c>
+      <c r="Q23" t="s">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="24" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A24" s="1" t="s">
-        <v>42</v>
+        <v>26</v>
       </c>
       <c r="B24" s="1" t="s">
-        <v>43</v>
+        <v>27</v>
       </c>
       <c r="C24">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E24" s="1" t="s">
-        <v>98</v>
+        <v>106</v>
       </c>
       <c r="F24" t="s">
-        <v>59</v>
+        <v>62</v>
       </c>
       <c r="G24">
         <v>0</v>
@@ -2447,27 +2456,27 @@
         <v>0</v>
       </c>
       <c r="N24">
-        <v>1</v>
-      </c>
-      <c r="O24" t="s">
-        <v>95</v>
-      </c>
-    </row>
-    <row r="25" spans="1:16" x14ac:dyDescent="0.3">
+        <v>0</v>
+      </c>
+      <c r="Q24" t="s">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="25" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A25" s="1" t="s">
-        <v>16</v>
+        <v>10</v>
       </c>
       <c r="B25" s="1" t="s">
-        <v>45</v>
+        <v>11</v>
       </c>
       <c r="C25">
         <v>1</v>
       </c>
       <c r="D25" s="1" t="s">
-        <v>85</v>
+        <v>87</v>
       </c>
       <c r="E25" s="1" t="s">
-        <v>98</v>
+        <v>109</v>
       </c>
       <c r="F25" t="s">
         <v>62</v>
@@ -2476,13 +2485,13 @@
         <v>0</v>
       </c>
       <c r="H25">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="I25">
         <v>0</v>
       </c>
       <c r="K25">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="L25">
         <v>0</v>
@@ -2493,31 +2502,31 @@
       <c r="N25">
         <v>0</v>
       </c>
-      <c r="P25" t="s">
-        <v>93</v>
-      </c>
-    </row>
-    <row r="26" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="Q25" t="s">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="26" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A26" s="1" t="s">
-        <v>18</v>
+        <v>8</v>
       </c>
       <c r="B26" s="1" t="s">
-        <v>47</v>
+        <v>9</v>
       </c>
       <c r="C26">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D26" s="1" t="s">
-        <v>85</v>
+        <v>87</v>
       </c>
       <c r="E26" s="1" t="s">
-        <v>98</v>
+        <v>108</v>
       </c>
       <c r="F26" t="s">
-        <v>59</v>
+        <v>62</v>
       </c>
       <c r="G26">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="H26">
         <v>0</v>
@@ -2537,60 +2546,57 @@
       <c r="N26">
         <v>0</v>
       </c>
-      <c r="P26" t="s">
-        <v>93</v>
-      </c>
-    </row>
-    <row r="27" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="Q26" t="s">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="27" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A27" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="B27" s="1" t="s">
+        <v>52</v>
+      </c>
+      <c r="C27">
+        <v>1</v>
+      </c>
+      <c r="E27" s="1" t="s">
+        <v>110</v>
+      </c>
+      <c r="F27" t="s">
+        <v>62</v>
+      </c>
+      <c r="G27">
+        <v>0</v>
+      </c>
+      <c r="H27">
+        <v>0</v>
+      </c>
+      <c r="I27">
+        <v>0</v>
+      </c>
+      <c r="K27">
+        <v>0</v>
+      </c>
+      <c r="L27">
+        <v>0</v>
+      </c>
+      <c r="M27">
+        <v>0</v>
+      </c>
+      <c r="N27">
+        <v>0</v>
+      </c>
+      <c r="Q27" t="s">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="28" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A28" s="1" t="s">
         <v>48</v>
       </c>
-      <c r="B27" s="1" t="s">
+      <c r="B28" s="1" t="s">
         <v>49</v>
-      </c>
-      <c r="C27">
-        <v>1</v>
-      </c>
-      <c r="D27" s="1" t="s">
-        <v>85</v>
-      </c>
-      <c r="E27" s="1" t="s">
-        <v>112</v>
-      </c>
-      <c r="F27" t="s">
-        <v>62</v>
-      </c>
-      <c r="G27">
-        <v>0</v>
-      </c>
-      <c r="H27">
-        <v>0</v>
-      </c>
-      <c r="I27">
-        <v>0</v>
-      </c>
-      <c r="K27">
-        <v>0</v>
-      </c>
-      <c r="L27">
-        <v>0</v>
-      </c>
-      <c r="M27">
-        <v>0</v>
-      </c>
-      <c r="N27">
-        <v>0</v>
-      </c>
-      <c r="P27" t="s">
-        <v>93</v>
-      </c>
-    </row>
-    <row r="28" spans="1:16" x14ac:dyDescent="0.3">
-      <c r="A28" s="1" t="s">
-        <v>50</v>
-      </c>
-      <c r="B28" s="1" t="s">
-        <v>51</v>
       </c>
       <c r="C28">
         <v>1</v>
@@ -2599,7 +2605,7 @@
         <v>85</v>
       </c>
       <c r="E28" s="1" t="s">
-        <v>98</v>
+        <v>112</v>
       </c>
       <c r="F28" t="s">
         <v>62</v>
@@ -2629,11 +2635,16 @@
         <v>93</v>
       </c>
     </row>
-    <row r="40" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="40" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A40" s="1"/>
       <c r="B40" s="1"/>
     </row>
   </sheetData>
+  <autoFilter ref="A1:R1" xr:uid="{387E2F34-DA14-4775-B5D9-5CA411BAE8BD}">
+    <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:R28">
+      <sortCondition ref="E1"/>
+    </sortState>
+  </autoFilter>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>